<commit_message>
Vocab terms now refer to distractor terms by number
</commit_message>
<xml_diff>
--- a/spec/fixtures/sample_vocab_terms.xlsx
+++ b/spec/fixtures/sample_vocab_terms.xlsx
@@ -126,9 +126,6 @@
     <t>Book</t>
   </si>
   <si>
-    <t>Prog</t>
-  </si>
-  <si>
     <t>Module UUID</t>
   </si>
   <si>
@@ -139,6 +136,9 @@
   </si>
   <si>
     <t>0d195918-0fda-42cd-b6e1-878a1a8e1c0a</t>
+  </si>
+  <si>
+    <t>Introduction to Programming</t>
   </si>
 </sst>
 </file>
@@ -546,11 +546,12 @@
     <sheetView tabSelected="1" showOutlineSymbols="0" showWhiteSpace="0" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="D2" sqref="D2"/>
-      <selection pane="bottomLeft" activeCell="D9" sqref="D9"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2:A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="13" x14ac:dyDescent="0"/>
   <cols>
+    <col min="1" max="1" width="21" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="6.5703125" style="5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="30.5703125" style="5" bestFit="1" customWidth="1"/>
@@ -571,7 +572,7 @@
         <v>1</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>2</v>
@@ -594,7 +595,7 @@
     </row>
     <row r="2" spans="1:10">
       <c r="A2" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="B2" s="3">
         <v>1</v>
@@ -603,7 +604,7 @@
         <v>8</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E2" t="s">
         <v>11</v>
@@ -626,7 +627,7 @@
     </row>
     <row r="3" spans="1:10">
       <c r="A3" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="B3" s="3">
         <v>2</v>
@@ -635,7 +636,7 @@
         <v>8</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E3" t="s">
         <v>12</v>
@@ -658,7 +659,7 @@
     </row>
     <row r="4" spans="1:10">
       <c r="A4" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="B4" s="3">
         <v>3</v>
@@ -667,7 +668,7 @@
         <v>8</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E4" t="s">
         <v>13</v>
@@ -690,7 +691,7 @@
     </row>
     <row r="5" spans="1:10">
       <c r="A5" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="B5" s="3">
         <v>4</v>
@@ -699,7 +700,7 @@
         <v>8</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E5" t="s">
         <v>14</v>
@@ -722,7 +723,7 @@
     </row>
     <row r="6" spans="1:10">
       <c r="A6" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="B6" s="3">
         <v>5</v>
@@ -731,7 +732,7 @@
         <v>9</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E6" t="s">
         <v>15</v>
@@ -754,7 +755,7 @@
     </row>
     <row r="7" spans="1:10">
       <c r="A7" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="B7" s="3">
         <v>6</v>
@@ -763,7 +764,7 @@
         <v>9</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E7" t="s">
         <v>16</v>
@@ -786,7 +787,7 @@
     </row>
     <row r="8" spans="1:10">
       <c r="A8" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="B8" s="3">
         <v>7</v>
@@ -795,7 +796,7 @@
         <v>10</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E8" t="s">
         <v>17</v>
@@ -818,7 +819,7 @@
     </row>
     <row r="9" spans="1:10">
       <c r="A9" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="B9" s="3">
         <v>8</v>
@@ -827,7 +828,7 @@
         <v>10</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E9" t="s">
         <v>18</v>

</xml_diff>